<commit_message>
Estimacion + pesos en CU
</commit_message>
<xml_diff>
--- a/Documentacion/EA/_ESTIMACIÓN.xlsx
+++ b/Documentacion/EA/_ESTIMACIÓN.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Facundo\Documents\GitHub\Mantenimiento\Documentacion\EA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Facundo\Desktop\Repositorio\Documentacion\EA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="231">
   <si>
     <t>Ponderación de Actores</t>
   </si>
@@ -102,9 +102,6 @@
     <t>Tabla 1 - Factores Técnicos TCF</t>
   </si>
   <si>
-    <t xml:space="preserve">complejo </t>
-  </si>
-  <si>
     <t>Factor</t>
   </si>
   <si>
@@ -129,9 +126,6 @@
     <t>No existe este tipo de funciones en la aplicación.</t>
   </si>
   <si>
-    <t>complejo</t>
-  </si>
-  <si>
     <t>T2</t>
   </si>
   <si>
@@ -159,12 +153,6 @@
     <t>T4</t>
   </si>
   <si>
-    <t>Procesamiento interno complejo</t>
-  </si>
-  <si>
-    <t>Algunos procesos complejos</t>
-  </si>
-  <si>
     <t>CU001.003.002 Modificacion de Usuario</t>
   </si>
   <si>
@@ -204,12 +192,6 @@
     <t>No se requiere portabilidad</t>
   </si>
   <si>
-    <t>CU001.004 Log-in de Usuario</t>
-  </si>
-  <si>
-    <t>medio</t>
-  </si>
-  <si>
     <t>T9</t>
   </si>
   <si>
@@ -219,9 +201,6 @@
     <t>No existe ninguna especificacion</t>
   </si>
   <si>
-    <t>CU001.005 Log-out de Usuario</t>
-  </si>
-  <si>
     <t>T10</t>
   </si>
   <si>
@@ -231,9 +210,6 @@
     <t>Se conoce el período punta diario.</t>
   </si>
   <si>
-    <t>CU001.006 Administracion de Personas</t>
-  </si>
-  <si>
     <t>TF11</t>
   </si>
   <si>
@@ -243,9 +219,6 @@
     <t>Seguridad normal</t>
   </si>
   <si>
-    <t>CU001.006.001 Agregar Persona</t>
-  </si>
-  <si>
     <t>T12</t>
   </si>
   <si>
@@ -255,9 +228,6 @@
     <t>Sólo accedido por  usuario administrador y usuario normal</t>
   </si>
   <si>
-    <t>CU001.006.002 Modificacion de Persona</t>
-  </si>
-  <si>
     <t>T13</t>
   </si>
   <si>
@@ -267,9 +237,6 @@
     <t>No se requiere entrenamiento especial, fácil de usar</t>
   </si>
   <si>
-    <t>CU001.006.003 Baja de Persona</t>
-  </si>
-  <si>
     <t>Total Factor Ajuste</t>
   </si>
   <si>
@@ -357,9 +324,6 @@
     <t>E7</t>
   </si>
   <si>
-    <t>Personal de medio tiempo</t>
-  </si>
-  <si>
     <t>Todos part-time</t>
   </si>
   <si>
@@ -387,69 +351,30 @@
     <t>Cálculos finales</t>
   </si>
   <si>
-    <t>CU004.001.002 Modificación de Pedidos</t>
-  </si>
-  <si>
     <t>Factor de complejidad técnica</t>
   </si>
   <si>
-    <t>CU004.001.003 Emisión de Pedidos</t>
-  </si>
-  <si>
     <t xml:space="preserve">TFC = </t>
   </si>
   <si>
-    <t>CU004.001.004 Buscar Pedido</t>
-  </si>
-  <si>
     <t>CU004.001.005 Visualizar Pedidos</t>
   </si>
   <si>
     <t>Factor de ambiente</t>
   </si>
   <si>
-    <t>CU004.001.006 Cargar Tarea</t>
-  </si>
-  <si>
     <t>EF=</t>
   </si>
   <si>
-    <t>CU004.001.007 Modificar Tarea</t>
-  </si>
-  <si>
-    <t>CU004.001.008 Quitar tarea</t>
-  </si>
-  <si>
-    <t>CU004.001.009 Visualizar Tarea</t>
-  </si>
-  <si>
-    <t>CU004.001.010 Asignar Insumo.</t>
-  </si>
-  <si>
-    <t>CU004.001.011 Asignar Agente</t>
-  </si>
-  <si>
-    <t>simple</t>
-  </si>
-  <si>
-    <t>CU004.001.012 Visualizar Historial</t>
-  </si>
-  <si>
     <t>Gestion de Insumos</t>
   </si>
   <si>
     <t>CU005.001 Administracion de Insumos.</t>
   </si>
   <si>
-    <t>CU005.001.002 Alta de Insumo</t>
-  </si>
-  <si>
     <t>CU005.001.003 Baja de Insumo</t>
   </si>
   <si>
-    <t>CU005.001.004 Modificacion de Insumo</t>
-  </si>
-  <si>
     <t>Gestion de Informes</t>
   </si>
   <si>
@@ -459,12 +384,6 @@
     <t>Puntos de casos de uso ajustados</t>
   </si>
   <si>
-    <t>CU006.001.001 Informe sobre reparaciones por sector</t>
-  </si>
-  <si>
-    <t>CU006.001.002 Informe sobre insumos por sector</t>
-  </si>
-  <si>
     <t>De E1 a E6 &lt;3 =</t>
   </si>
   <si>
@@ -498,18 +417,12 @@
     <t>Diseño</t>
   </si>
   <si>
-    <t>Gestion de Actividades</t>
-  </si>
-  <si>
     <t>CF</t>
   </si>
   <si>
     <t>Desarrollo</t>
   </si>
   <si>
-    <t>CU007.001 Administracion de Calendario de Actividades</t>
-  </si>
-  <si>
     <t>Pruebas</t>
   </si>
   <si>
@@ -537,54 +450,24 @@
     <t>CU007.001.004 Búsqueda de Evento</t>
   </si>
   <si>
-    <t>CU007.001.005 Visualizar evento</t>
-  </si>
-  <si>
     <t>Gestion de Especializacion</t>
   </si>
   <si>
     <t>CU008.001 Administracion de especializacion</t>
   </si>
   <si>
-    <t>CU008.001.001 Crear especializacion</t>
-  </si>
-  <si>
-    <t>CU008.001.002 Eliminar especializacion</t>
-  </si>
-  <si>
     <t>Gestion de Ordenes de Compra</t>
   </si>
   <si>
     <t>CU009.001 Administracion de Ordenes de Compra</t>
   </si>
   <si>
-    <t>CU009.001.001 Visualizar Orden de Compra</t>
-  </si>
-  <si>
-    <t>CU009.001.003 Generar Orden de Compra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">medio </t>
-  </si>
-  <si>
     <t>Gestion de orden de Trabajo</t>
   </si>
   <si>
     <t>CU010.001 Gestion de Ordenes de Trabajo</t>
   </si>
   <si>
-    <t>CU010.001.001 Creacion de Orden de Trabajo</t>
-  </si>
-  <si>
-    <t>CU010.001.002 Modificacion de Orden de Trabajo</t>
-  </si>
-  <si>
-    <t>CU010.001.003 Visualizar Orden de Trabajo</t>
-  </si>
-  <si>
-    <t>CU010.001.004 Buscar Orden de Trabajo</t>
-  </si>
-  <si>
     <t>CU010.001.005 Verificar Finalizacion de Orden de Trabajo</t>
   </si>
   <si>
@@ -633,25 +516,202 @@
     <t>CU001.003.004 Consulta Usuario</t>
   </si>
   <si>
-    <t>CU001.003.005 Asignación de Rol a Usuario</t>
-  </si>
-  <si>
-    <t>CU001.003.006 Emisión de listado de Usuario</t>
-  </si>
-  <si>
-    <t>CU001.003.007 Autenticar Usuario</t>
-  </si>
-  <si>
     <t>CU001.002.005.001 Asignación de permisos</t>
   </si>
   <si>
     <t>CU001.002.005.002 Desasignar permisos</t>
   </si>
   <si>
-    <t>CU001.003.005.001 Asignación de Rol a Usuario</t>
-  </si>
-  <si>
-    <t>CU001.003.005.002 Desasignar Rol a Usuario</t>
+    <t>CU001.003.001.001 Asignacion de roles a Usuario</t>
+  </si>
+  <si>
+    <t>CU001.003.005 Emision de Listado de Usuarios</t>
+  </si>
+  <si>
+    <t>CU001.003.006 Autenticar Usuario</t>
+  </si>
+  <si>
+    <t>CU001.003.006.001 Log-in de Usuario</t>
+  </si>
+  <si>
+    <t>CU001.003.006.002 Log-out de Usuario</t>
+  </si>
+  <si>
+    <t>CU001.004 Administracion de Personas</t>
+  </si>
+  <si>
+    <t>CU001.004.001 Alta de Persona</t>
+  </si>
+  <si>
+    <t>CU001.004.002 Modificacion de Persona</t>
+  </si>
+  <si>
+    <t>CU001.004.003 Baja de Persona</t>
+  </si>
+  <si>
+    <t>CU001.004.004 Consulta de Persona</t>
+  </si>
+  <si>
+    <t>CU001.004.005 Emision de listado de Personas</t>
+  </si>
+  <si>
+    <t>CU002.001.004 Consulta de Agente</t>
+  </si>
+  <si>
+    <t>CU002.001.003 Visualizar Agente</t>
+  </si>
+  <si>
+    <t>CU002.001.003 Emision de listado de Agentes</t>
+  </si>
+  <si>
+    <t>CU003.001.004 Consulta de Sectores</t>
+  </si>
+  <si>
+    <t>CU003.001.005 Emision de listado de Sectores</t>
+  </si>
+  <si>
+    <t>CU004.001.002 Consulta de Pedidos</t>
+  </si>
+  <si>
+    <t>CU004.001.003 Emision de listado de Pedidos</t>
+  </si>
+  <si>
+    <t>CU004.001.004 Modificar de Pedidos</t>
+  </si>
+  <si>
+    <t>CU004.001.005.002 Visualizar Tarea</t>
+  </si>
+  <si>
+    <t>CU004.001.005.002.001 Alta de Tarea</t>
+  </si>
+  <si>
+    <t>CU004.001.005.002.002 Agregar Recursos</t>
+  </si>
+  <si>
+    <t>CU004.001.004.003.001 Asignar Insumo</t>
+  </si>
+  <si>
+    <t>CU004.001.004.003.004 Asignar Agente</t>
+  </si>
+  <si>
+    <t>CU004.001.005.002.003 Quitar Recursos</t>
+  </si>
+  <si>
+    <t>CU004.001.005.002.004 Quitar Tarea</t>
+  </si>
+  <si>
+    <t>CU004.001.004.003.005 Quitar Agente</t>
+  </si>
+  <si>
+    <t>CU004.001.004.003.002 Quitar Insumo</t>
+  </si>
+  <si>
+    <t>CU004.001.005.002.005 Modificación de Tarea</t>
+  </si>
+  <si>
+    <t>CU004.001.005.002.006 Emisión de listado de Tarea</t>
+  </si>
+  <si>
+    <t>CU004.001.005.001 Visualizar Historial</t>
+  </si>
+  <si>
+    <t>CU004.001.005.001.001 Emisión de Historial de Pedidos</t>
+  </si>
+  <si>
+    <t>CU005.001.001 Alta de Insumo</t>
+  </si>
+  <si>
+    <t>CU005.001.002 Modificación de Insumo</t>
+  </si>
+  <si>
+    <t>CU005.001.004 Consulta de Insumo</t>
+  </si>
+  <si>
+    <t>CU005.001.005 Emisión de listado de Insumo</t>
+  </si>
+  <si>
+    <t>CU006.001.006 Consulta de historial de insumo</t>
+  </si>
+  <si>
+    <t>CU006.001.001 Informe sobre Pedidos</t>
+  </si>
+  <si>
+    <t>CU006.001.002 Informe sobre ordenes de Trabajo</t>
+  </si>
+  <si>
+    <t>Gestion de Eventos</t>
+  </si>
+  <si>
+    <t>CU007.001 Administracion de Calendario de Eventos</t>
+  </si>
+  <si>
+    <t>CU008.001.001 Alta de especializacion</t>
+  </si>
+  <si>
+    <t>CU008.001.002 Modificación de especializacion</t>
+  </si>
+  <si>
+    <t>CU008.001.003 Baja de especializacion</t>
+  </si>
+  <si>
+    <t>CU008.001.004 Consulta de especializacion</t>
+  </si>
+  <si>
+    <t>CU008.001.005 Emision de listado de especializaciones</t>
+  </si>
+  <si>
+    <t>CU009.001.001 Alta de Orden de Compra</t>
+  </si>
+  <si>
+    <t>CU009.001.002 Modificacion de Orden de Compra</t>
+  </si>
+  <si>
+    <t>CU009.001.003 Visualizar Orden de Compra</t>
+  </si>
+  <si>
+    <t>CU009.001.003.001 Sumar Entrada</t>
+  </si>
+  <si>
+    <t>CU009.001.003.002 Anular pedido de Insumo</t>
+  </si>
+  <si>
+    <t>CU009.001.003.003 Emision de Orden de Compra</t>
+  </si>
+  <si>
+    <t>CU009.001.004 Consulta de Orden de Compra</t>
+  </si>
+  <si>
+    <t>CU009.001.005 Emision de listado de orden de compra</t>
+  </si>
+  <si>
+    <t>CU010.001.001 Alta de Orden de Trabajo</t>
+  </si>
+  <si>
+    <t>CU010.001.002 Buscar Tarea</t>
+  </si>
+  <si>
+    <t>CU010.001.003 Emitir listado de Ordenes de Trabajo</t>
+  </si>
+  <si>
+    <t>CU010.001.004 Visualizar Orden de Trabajo</t>
+  </si>
+  <si>
+    <t>CU010.001.004.001 Emitir listado de tareas</t>
+  </si>
+  <si>
+    <t>CU010.001.004.002 Visualizar listado de tareas</t>
+  </si>
+  <si>
+    <t>Personal de Medio tiempo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medio </t>
+  </si>
+  <si>
+    <t>Procesamiento interno Complejo</t>
+  </si>
+  <si>
+    <t>Algunos procesos Complejos</t>
   </si>
 </sst>
 </file>
@@ -754,7 +814,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -903,11 +963,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1122,6 +1210,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1439,10 +1531,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P106"/>
+  <dimension ref="A1:P128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1596,7 +1688,7 @@
       </c>
       <c r="H7" s="13">
         <f>SUM(E9:E11)</f>
-        <v>820</v>
+        <v>865</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
@@ -1636,11 +1728,12 @@
         <v>5</v>
       </c>
       <c r="D9" s="19">
-        <v>8</v>
+        <f>COUNTIF(C15:C126,"Simple")</f>
+        <v>40</v>
       </c>
       <c r="E9" s="20">
         <f t="shared" ref="E9:E11" si="0">C9*D9</f>
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="12" t="s">
@@ -1648,7 +1741,7 @@
       </c>
       <c r="H9" s="13">
         <f>SUM(H5:H7)</f>
-        <v>826</v>
+        <v>871</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
@@ -1665,11 +1758,12 @@
         <v>10</v>
       </c>
       <c r="D10" s="19">
-        <v>18</v>
+        <f>COUNTIF(C15:C126,"Medio")</f>
+        <v>41</v>
       </c>
       <c r="E10" s="20">
         <f t="shared" si="0"/>
-        <v>180</v>
+        <v>410</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="14"/>
@@ -1689,11 +1783,12 @@
         <v>15</v>
       </c>
       <c r="D11" s="19">
-        <v>40</v>
+        <f>COUNTIF(C15:C126,"Complejo")</f>
+        <v>17</v>
       </c>
       <c r="E11" s="20">
         <f t="shared" si="0"/>
-        <v>600</v>
+        <v>255</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="12" t="s">
@@ -1701,7 +1796,7 @@
       </c>
       <c r="H11" s="22">
         <f>H9*G47*G50</f>
-        <v>653.38664999999992</v>
+        <v>688.98277499999983</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
@@ -1756,13 +1851,13 @@
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="27" t="s">
-        <v>189</v>
+        <v>150</v>
       </c>
       <c r="B15" s="19">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -1775,7 +1870,7 @@
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="27" t="s">
-        <v>190</v>
+        <v>151</v>
       </c>
       <c r="B16" s="19">
         <v>7</v>
@@ -1794,10 +1889,14 @@
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="85" t="s">
-        <v>191</v>
-      </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="28"/>
+        <v>152</v>
+      </c>
+      <c r="B17" s="20">
+        <v>4</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="D17" s="3"/>
       <c r="E17" s="29"/>
       <c r="F17" s="99" t="s">
@@ -1811,48 +1910,52 @@
     </row>
     <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="27" t="s">
-        <v>192</v>
+        <v>153</v>
       </c>
       <c r="B18" s="19">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="29"/>
       <c r="F18" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="H18" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="G18" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="H18" s="30" t="s">
+      <c r="I18" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="I18" s="31" t="s">
+      <c r="J18" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="J18" s="31" t="s">
+      <c r="K18" s="32" t="s">
         <v>31</v>
-      </c>
-      <c r="K18" s="32" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="85" t="s">
-        <v>193</v>
-      </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="28"/>
+        <v>154</v>
+      </c>
+      <c r="B19" s="20">
+        <v>2</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>6</v>
+      </c>
       <c r="D19" s="3"/>
       <c r="E19" s="29"/>
       <c r="F19" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" s="34" t="s">
         <v>33</v>
-      </c>
-      <c r="G19" s="34" t="s">
-        <v>34</v>
       </c>
       <c r="H19" s="35">
         <v>2</v>
@@ -1865,22 +1968,26 @@
         <v>0</v>
       </c>
       <c r="K19" s="36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="85" t="s">
-        <v>194</v>
-      </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="28"/>
+        <v>155</v>
+      </c>
+      <c r="B20" s="20">
+        <v>2</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>6</v>
+      </c>
       <c r="D20" s="3"/>
       <c r="E20" s="29"/>
       <c r="F20" s="33" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G20" s="34" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H20" s="37">
         <v>1</v>
@@ -1893,12 +2000,12 @@
         <v>3</v>
       </c>
       <c r="K20" s="38" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="27" t="s">
-        <v>195</v>
+        <v>156</v>
       </c>
       <c r="B21" s="19">
         <v>6</v>
@@ -1909,10 +2016,10 @@
       <c r="D21" s="3"/>
       <c r="E21" s="29"/>
       <c r="F21" s="33" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G21" s="34" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H21" s="37">
         <v>1</v>
@@ -1925,15 +2032,15 @@
         <v>2</v>
       </c>
       <c r="K21" s="42" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="27" t="s">
-        <v>196</v>
+        <v>157</v>
       </c>
       <c r="B22" s="19">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>8</v>
@@ -1941,10 +2048,10 @@
       <c r="D22" s="3"/>
       <c r="E22" s="29"/>
       <c r="F22" s="33" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G22" s="34" t="s">
-        <v>46</v>
+        <v>229</v>
       </c>
       <c r="H22" s="43">
         <v>1</v>
@@ -1957,15 +2064,15 @@
         <v>3</v>
       </c>
       <c r="K22" s="44" t="s">
-        <v>47</v>
+        <v>230</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="27" t="s">
-        <v>197</v>
+        <v>158</v>
       </c>
       <c r="B23" s="19">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23" s="28" t="s">
         <v>8</v>
@@ -1973,10 +2080,10 @@
       <c r="D23" s="3"/>
       <c r="E23" s="29"/>
       <c r="F23" s="33" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G23" s="34" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H23" s="37">
         <v>1</v>
@@ -1989,22 +2096,26 @@
         <v>2</v>
       </c>
       <c r="K23" s="42" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="85" t="s">
-        <v>198</v>
-      </c>
-      <c r="B24" s="20"/>
-      <c r="C24" s="28"/>
+        <v>159</v>
+      </c>
+      <c r="B24" s="20">
+        <v>4</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="D24" s="3"/>
       <c r="E24" s="29"/>
       <c r="F24" s="33" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G24" s="34" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="H24" s="37">
         <v>0.5</v>
@@ -2017,22 +2128,26 @@
         <v>0.5</v>
       </c>
       <c r="K24" s="44" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="85" t="s">
-        <v>199</v>
-      </c>
-      <c r="B25" s="20"/>
-      <c r="C25" s="28"/>
+        <v>160</v>
+      </c>
+      <c r="B25" s="20">
+        <v>2</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>6</v>
+      </c>
       <c r="D25" s="3"/>
       <c r="E25" s="29"/>
       <c r="F25" s="33" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G25" s="34" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H25" s="37">
         <v>0.5</v>
@@ -2045,22 +2160,22 @@
         <v>2</v>
       </c>
       <c r="K25" s="42" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="85" t="s">
-        <v>200</v>
+        <v>161</v>
       </c>
       <c r="B26" s="20"/>
       <c r="C26" s="28"/>
       <c r="D26" s="3"/>
       <c r="E26" s="29"/>
       <c r="F26" s="33" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G26" s="34" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H26" s="37">
         <v>2</v>
@@ -2073,22 +2188,22 @@
         <v>2</v>
       </c>
       <c r="K26" s="42" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="85" t="s">
-        <v>207</v>
+        <v>165</v>
       </c>
       <c r="B27" s="20"/>
       <c r="C27" s="28"/>
       <c r="D27" s="3"/>
       <c r="E27" s="29"/>
       <c r="F27" s="33" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G27" s="34" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H27" s="37">
         <v>1</v>
@@ -2101,22 +2216,22 @@
         <v>0</v>
       </c>
       <c r="K27" s="44" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="85" t="s">
-        <v>208</v>
+        <v>166</v>
       </c>
       <c r="B28" s="20"/>
       <c r="C28" s="28"/>
       <c r="D28" s="3"/>
       <c r="E28" s="29"/>
       <c r="F28" s="33" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G28" s="34" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="H28" s="43">
         <v>1</v>
@@ -2129,22 +2244,26 @@
         <v>1</v>
       </c>
       <c r="K28" s="44" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="85" t="s">
-        <v>201</v>
-      </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="28"/>
+        <v>162</v>
+      </c>
+      <c r="B29" s="20">
+        <v>2</v>
+      </c>
+      <c r="C29" s="28" t="s">
+        <v>6</v>
+      </c>
       <c r="D29" s="3"/>
       <c r="E29" s="29"/>
       <c r="F29" s="46" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="G29" s="47" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="H29" s="37">
         <v>1</v>
@@ -2157,26 +2276,26 @@
         <v>1</v>
       </c>
       <c r="K29" s="38" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="39" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B30" s="40">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C30" s="41" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="29"/>
       <c r="F30" s="33" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="G30" s="34" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="H30" s="37">
         <v>1</v>
@@ -2189,26 +2308,26 @@
         <v>0</v>
       </c>
       <c r="K30" s="44" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="27" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B31" s="19">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="29"/>
       <c r="F31" s="33" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G31" s="34" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="H31" s="43">
         <v>1</v>
@@ -2221,23 +2340,23 @@
         <v>3</v>
       </c>
       <c r="K31" s="42" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="B32" s="19">
-        <v>6</v>
+      <c r="A32" s="85" t="s">
+        <v>167</v>
+      </c>
+      <c r="B32" s="20">
+        <v>2</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="29"/>
       <c r="F32" s="48" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="G32" s="49"/>
       <c r="H32" s="49"/>
@@ -2250,13 +2369,13 @@
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="27" t="s">
-        <v>202</v>
+        <v>44</v>
       </c>
       <c r="B33" s="19">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="29"/>
@@ -2269,18 +2388,18 @@
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="27" t="s">
-        <v>203</v>
+        <v>163</v>
       </c>
       <c r="B34" s="19">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C34" s="28" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="29"/>
       <c r="F34" s="99" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="G34" s="100"/>
       <c r="H34" s="100"/>
@@ -2290,10 +2409,10 @@
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="27" t="s">
-        <v>204</v>
+        <v>164</v>
       </c>
       <c r="B35" s="19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C35" s="28" t="s">
         <v>6</v>
@@ -2301,10 +2420,10 @@
       <c r="D35" s="3"/>
       <c r="E35" s="29"/>
       <c r="F35" s="33" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="G35" s="34" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="H35" s="53">
         <v>1.5</v>
@@ -2317,22 +2436,26 @@
         <v>4.5</v>
       </c>
       <c r="K35" s="54" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="85" t="s">
-        <v>209</v>
-      </c>
-      <c r="B36" s="20"/>
-      <c r="C36" s="28"/>
+      <c r="A36" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="B36" s="19">
+        <v>3</v>
+      </c>
+      <c r="C36" s="28" t="s">
+        <v>6</v>
+      </c>
       <c r="D36" s="3"/>
       <c r="E36" s="29"/>
       <c r="F36" s="33" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="G36" s="34" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="H36" s="37">
         <v>0.5</v>
@@ -2345,22 +2468,22 @@
         <v>1.5</v>
       </c>
       <c r="K36" s="55" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="85" t="s">
-        <v>210</v>
+        <v>169</v>
       </c>
       <c r="B37" s="20"/>
       <c r="C37" s="28"/>
       <c r="D37" s="3"/>
       <c r="E37" s="29"/>
       <c r="F37" s="33" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="G37" s="34" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="H37" s="37">
         <v>1</v>
@@ -2373,22 +2496,26 @@
         <v>3</v>
       </c>
       <c r="K37" s="54" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="85" t="s">
-        <v>205</v>
-      </c>
-      <c r="B38" s="20"/>
-      <c r="C38" s="28"/>
+      <c r="A38" s="98" t="s">
+        <v>170</v>
+      </c>
+      <c r="B38" s="45">
+        <v>4</v>
+      </c>
+      <c r="C38" s="45" t="s">
+        <v>8</v>
+      </c>
       <c r="D38" s="3"/>
       <c r="E38" s="29"/>
       <c r="F38" s="33" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="G38" s="34" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="H38" s="37">
         <v>0.5</v>
@@ -2401,22 +2528,26 @@
         <v>1.5</v>
       </c>
       <c r="K38" s="55" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="85" t="s">
-        <v>206</v>
-      </c>
-      <c r="B39" s="20"/>
-      <c r="C39" s="28"/>
+      <c r="A39" s="98" t="s">
+        <v>171</v>
+      </c>
+      <c r="B39" s="45">
+        <v>1</v>
+      </c>
+      <c r="C39" s="98" t="s">
+        <v>6</v>
+      </c>
       <c r="D39" s="3"/>
       <c r="E39" s="29"/>
       <c r="F39" s="43" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="G39" s="34" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="H39" s="37">
         <v>1</v>
@@ -2429,26 +2560,24 @@
         <v>5</v>
       </c>
       <c r="K39" s="54" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="45" t="s">
-        <v>61</v>
-      </c>
-      <c r="B40" s="45">
-        <v>6</v>
-      </c>
-      <c r="C40" s="45" t="s">
-        <v>62</v>
+      <c r="A40" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="B40" s="19"/>
+      <c r="C40" s="28" t="s">
+        <v>11</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="29"/>
       <c r="F40" s="43" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="G40" s="34" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="H40" s="37">
         <v>2</v>
@@ -2461,26 +2590,26 @@
         <v>6</v>
       </c>
       <c r="K40" s="54" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="45" t="s">
-        <v>66</v>
-      </c>
-      <c r="B41" s="45">
-        <v>5</v>
-      </c>
-      <c r="C41" s="45" t="s">
-        <v>62</v>
+      <c r="A41" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="B41" s="19">
+        <v>8</v>
+      </c>
+      <c r="C41" s="28" t="s">
+        <v>11</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="33" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="G41" s="34" t="s">
-        <v>112</v>
+        <v>227</v>
       </c>
       <c r="H41" s="37">
         <v>-1</v>
@@ -2493,26 +2622,26 @@
         <v>-5</v>
       </c>
       <c r="K41" s="55" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="27" t="s">
-        <v>70</v>
+        <v>174</v>
       </c>
       <c r="B42" s="19">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C42" s="28" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="29"/>
       <c r="F42" s="33" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="G42" s="34" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="H42" s="37">
         <v>-1</v>
@@ -2525,23 +2654,23 @@
         <v>-3</v>
       </c>
       <c r="K42" s="54" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
     </row>
     <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="27" t="s">
-        <v>74</v>
+        <v>175</v>
       </c>
       <c r="B43" s="19">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C43" s="28" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="29"/>
       <c r="F43" s="48" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="G43" s="49"/>
       <c r="H43" s="49"/>
@@ -2553,14 +2682,14 @@
       <c r="K43" s="49"/>
     </row>
     <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="B44" s="19">
-        <v>10</v>
+      <c r="A44" s="85" t="s">
+        <v>176</v>
+      </c>
+      <c r="B44" s="20">
+        <v>2</v>
       </c>
       <c r="C44" s="28" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="29"/>
@@ -2572,19 +2701,19 @@
       <c r="K44" s="3"/>
     </row>
     <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="B45" s="19">
-        <v>10</v>
+      <c r="A45" s="85" t="s">
+        <v>177</v>
+      </c>
+      <c r="B45" s="20">
+        <v>2</v>
       </c>
       <c r="C45" s="28" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="104" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="G45" s="105"/>
       <c r="H45" s="3"/>
@@ -2592,14 +2721,14 @@
     </row>
     <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="51" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B46" s="26"/>
       <c r="C46" s="26"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="57" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="G46" s="58"/>
       <c r="H46" s="3"/>
@@ -2608,18 +2737,18 @@
     </row>
     <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="27" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="B47" s="19">
         <v>8</v>
       </c>
       <c r="C47" s="28" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
       <c r="F47" s="60" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="G47" s="61">
         <f>0.6+(0.01*J32)</f>
@@ -2632,13 +2761,13 @@
     </row>
     <row r="48" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="27" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B48" s="19">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C48" s="28" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
@@ -2651,18 +2780,18 @@
     </row>
     <row r="49" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="27" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="B49" s="19">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C49" s="28" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
       <c r="F49" s="57" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="G49" s="63"/>
       <c r="H49" s="3"/>
@@ -2673,18 +2802,18 @@
     </row>
     <row r="50" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="27" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B50" s="19">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C50" s="28" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
       <c r="F50" s="67" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="G50" s="68">
         <f>1.4 - 0.03*J43</f>
@@ -2696,11 +2825,15 @@
       <c r="P50" s="3"/>
     </row>
     <row r="51" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="51" t="s">
-        <v>99</v>
-      </c>
-      <c r="B51" s="26"/>
-      <c r="C51" s="26"/>
+      <c r="A51" s="85" t="s">
+        <v>178</v>
+      </c>
+      <c r="B51" s="20">
+        <v>2</v>
+      </c>
+      <c r="C51" s="28" t="s">
+        <v>6</v>
+      </c>
       <c r="D51" s="69"/>
       <c r="E51" s="3"/>
       <c r="F51" s="70"/>
@@ -2713,14 +2846,14 @@
       <c r="P51" s="3"/>
     </row>
     <row r="52" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="27" t="s">
-        <v>102</v>
-      </c>
-      <c r="B52" s="19">
-        <v>10</v>
+      <c r="A52" s="85" t="s">
+        <v>179</v>
+      </c>
+      <c r="B52" s="20">
+        <v>2</v>
       </c>
       <c r="C52" s="28" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D52" s="69"/>
       <c r="E52" s="3"/>
@@ -2734,14 +2867,14 @@
       <c r="P52" s="3"/>
     </row>
     <row r="53" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="27" t="s">
-        <v>106</v>
-      </c>
-      <c r="B53" s="19">
-        <v>8</v>
+      <c r="A53" s="85" t="s">
+        <v>180</v>
+      </c>
+      <c r="B53" s="20">
+        <v>2</v>
       </c>
       <c r="C53" s="28" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D53" s="69"/>
       <c r="E53" s="3"/>
@@ -2755,15 +2888,11 @@
       <c r="P53" s="3"/>
     </row>
     <row r="54" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="B54" s="19">
-        <v>8</v>
-      </c>
-      <c r="C54" s="28" t="s">
-        <v>36</v>
-      </c>
+      <c r="A54" s="51" t="s">
+        <v>88</v>
+      </c>
+      <c r="B54" s="26"/>
+      <c r="C54" s="26"/>
       <c r="D54" s="69"/>
       <c r="E54" s="3"/>
       <c r="F54" s="70"/>
@@ -2777,13 +2906,13 @@
     </row>
     <row r="55" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="27" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="B55" s="19">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C55" s="28" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D55" s="69"/>
       <c r="E55" s="3"/>
@@ -2797,11 +2926,15 @@
       <c r="P55" s="3"/>
     </row>
     <row r="56" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="51" t="s">
-        <v>118</v>
-      </c>
-      <c r="B56" s="26"/>
-      <c r="C56" s="26"/>
+      <c r="A56" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="B56" s="19">
+        <v>9</v>
+      </c>
+      <c r="C56" s="28" t="s">
+        <v>11</v>
+      </c>
       <c r="D56" s="69"/>
       <c r="E56" s="3"/>
       <c r="F56" s="70"/>
@@ -2815,13 +2948,13 @@
     </row>
     <row r="57" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="27" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="B57" s="19">
+        <v>8</v>
+      </c>
+      <c r="C57" s="28" t="s">
         <v>11</v>
-      </c>
-      <c r="C57" s="28" t="s">
-        <v>36</v>
       </c>
       <c r="D57" s="69"/>
       <c r="E57" s="3"/>
@@ -2836,13 +2969,13 @@
     </row>
     <row r="58" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="27" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="B58" s="19">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C58" s="28" t="s">
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="D58" s="69"/>
       <c r="E58" s="3"/>
@@ -2856,14 +2989,14 @@
       <c r="P58" s="3"/>
     </row>
     <row r="59" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="B59" s="19">
-        <v>16</v>
+      <c r="A59" s="85" t="s">
+        <v>181</v>
+      </c>
+      <c r="B59" s="20">
+        <v>2</v>
       </c>
       <c r="C59" s="28" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
@@ -2877,14 +3010,14 @@
       <c r="P59" s="3"/>
     </row>
     <row r="60" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="27" t="s">
-        <v>124</v>
-      </c>
-      <c r="B60" s="19">
-        <v>10</v>
+      <c r="A60" s="85" t="s">
+        <v>182</v>
+      </c>
+      <c r="B60" s="20">
+        <v>2</v>
       </c>
       <c r="C60" s="28" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
@@ -2898,15 +3031,11 @@
       <c r="P60" s="3"/>
     </row>
     <row r="61" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="B61" s="19">
-        <v>3</v>
-      </c>
-      <c r="C61" s="28" t="s">
-        <v>6</v>
-      </c>
+      <c r="A61" s="51" t="s">
+        <v>106</v>
+      </c>
+      <c r="B61" s="26"/>
+      <c r="C61" s="26"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
       <c r="F61" s="76"/>
@@ -2921,13 +3050,13 @@
     </row>
     <row r="62" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="27" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="B62" s="19">
         <v>8</v>
       </c>
       <c r="C62" s="28" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
@@ -2940,19 +3069,19 @@
       <c r="P62" s="3"/>
     </row>
     <row r="63" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="65" t="s">
-        <v>129</v>
-      </c>
-      <c r="B63" s="66">
-        <v>8</v>
-      </c>
-      <c r="C63" s="66" t="s">
-        <v>36</v>
+      <c r="A63" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="B63" s="19">
+        <v>7</v>
+      </c>
+      <c r="C63" s="28" t="s">
+        <v>8</v>
       </c>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
       <c r="F63" s="80" t="s">
-        <v>145</v>
+        <v>120</v>
       </c>
       <c r="G63" s="77"/>
       <c r="H63" s="3"/>
@@ -2962,14 +3091,14 @@
       <c r="P63" s="3"/>
     </row>
     <row r="64" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="65" t="s">
-        <v>131</v>
-      </c>
-      <c r="B64" s="66">
-        <v>5</v>
-      </c>
-      <c r="C64" s="66" t="s">
-        <v>62</v>
+      <c r="A64" s="85" t="s">
+        <v>183</v>
+      </c>
+      <c r="B64" s="20">
+        <v>2</v>
+      </c>
+      <c r="C64" s="28" t="s">
+        <v>6</v>
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
@@ -2981,233 +3110,237 @@
       <c r="P64" s="3"/>
     </row>
     <row r="65" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="65" t="s">
-        <v>132</v>
-      </c>
-      <c r="B65" s="66">
-        <v>6</v>
-      </c>
-      <c r="C65" s="66" t="s">
-        <v>62</v>
+      <c r="A65" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B65" s="19">
+        <v>2</v>
+      </c>
+      <c r="C65" s="28" t="s">
+        <v>6</v>
       </c>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
       <c r="F65" s="81" t="s">
-        <v>148</v>
+        <v>121</v>
       </c>
       <c r="G65" s="82">
         <f>COUNTIF(I35:I40,"&lt;3")</f>
         <v>0</v>
       </c>
       <c r="H65" s="83" t="s">
-        <v>149</v>
+        <v>122</v>
       </c>
       <c r="I65" s="83" t="s">
-        <v>150</v>
+        <v>123</v>
       </c>
       <c r="J65" s="84" t="s">
-        <v>151</v>
+        <v>124</v>
       </c>
       <c r="K65" s="84" t="s">
-        <v>152</v>
+        <v>125</v>
       </c>
     </row>
     <row r="66" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="45" t="s">
-        <v>133</v>
-      </c>
-      <c r="B66" s="45">
-        <v>11</v>
-      </c>
-      <c r="C66" s="45" t="s">
-        <v>36</v>
+      <c r="A66" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B66" s="19">
+        <v>7</v>
+      </c>
+      <c r="C66" s="28" t="s">
+        <v>8</v>
       </c>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
       <c r="F66" s="81" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="G66" s="82">
         <f>COUNTIF(I41:I42,"&gt;3")</f>
         <v>1</v>
       </c>
       <c r="H66" s="85" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="I66" s="86">
         <v>0.1</v>
       </c>
       <c r="J66" s="87">
         <f t="shared" ref="J66:J67" si="3">I66*J67/I67</f>
-        <v>1633.4666249999998</v>
+        <v>1722.4569374999999</v>
       </c>
       <c r="K66" s="87">
         <f t="shared" ref="K66:K70" si="4">J66/8</f>
-        <v>204.18332812499997</v>
+        <v>215.30711718749998</v>
       </c>
     </row>
     <row r="67" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="65" t="s">
-        <v>134</v>
-      </c>
-      <c r="B67" s="66">
-        <v>5</v>
-      </c>
-      <c r="C67" s="66" t="s">
-        <v>62</v>
+      <c r="A67" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="B67" s="19">
+        <v>4</v>
+      </c>
+      <c r="C67" s="28" t="s">
+        <v>8</v>
       </c>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
       <c r="F67" s="88" t="s">
-        <v>157</v>
+        <v>130</v>
       </c>
       <c r="G67" s="89">
         <f>SUM(G65:G66)</f>
         <v>1</v>
       </c>
       <c r="H67" s="85" t="s">
-        <v>158</v>
+        <v>131</v>
       </c>
       <c r="I67" s="86">
         <v>0.2</v>
       </c>
       <c r="J67" s="87">
         <f t="shared" si="3"/>
-        <v>3266.9332499999996</v>
+        <v>3444.9138749999997</v>
       </c>
       <c r="K67" s="87">
         <f t="shared" si="4"/>
-        <v>408.36665624999995</v>
+        <v>430.61423437499997</v>
       </c>
     </row>
     <row r="68" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="65" t="s">
-        <v>135</v>
-      </c>
-      <c r="B68" s="66">
-        <v>3</v>
-      </c>
-      <c r="C68" s="66" t="s">
-        <v>136</v>
+      <c r="A68" s="85" t="s">
+        <v>186</v>
+      </c>
+      <c r="B68" s="20">
+        <v>8</v>
+      </c>
+      <c r="C68" s="28" t="s">
+        <v>11</v>
       </c>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
       <c r="F68" s="88" t="s">
-        <v>160</v>
+        <v>132</v>
       </c>
       <c r="G68" s="82">
         <f>G67*10</f>
         <v>10</v>
       </c>
       <c r="H68" s="85" t="s">
-        <v>161</v>
+        <v>133</v>
       </c>
       <c r="I68" s="90">
         <v>0.4</v>
       </c>
       <c r="J68" s="91">
         <f>G71</f>
-        <v>6533.8664999999992</v>
+        <v>6889.8277499999986</v>
       </c>
       <c r="K68" s="91">
         <f t="shared" si="4"/>
-        <v>816.7333124999999</v>
+        <v>861.22846874999982</v>
       </c>
     </row>
     <row r="69" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="65" t="s">
-        <v>137</v>
+        <v>187</v>
       </c>
       <c r="B69" s="66">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C69" s="66" t="s">
-        <v>136</v>
+        <v>8</v>
       </c>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
       <c r="F69" s="62"/>
       <c r="G69" s="63"/>
       <c r="H69" s="85" t="s">
-        <v>163</v>
+        <v>134</v>
       </c>
       <c r="I69" s="86">
         <v>0.15</v>
       </c>
       <c r="J69" s="87">
         <f t="shared" ref="J69:J70" si="5">I69*J68/I68</f>
-        <v>2450.1999374999996</v>
+        <v>2583.6854062499992</v>
       </c>
       <c r="K69" s="87">
         <f t="shared" si="4"/>
-        <v>306.27499218749995</v>
+        <v>322.9606757812499</v>
       </c>
     </row>
     <row r="70" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="51" t="s">
-        <v>138</v>
-      </c>
-      <c r="B70" s="26"/>
-      <c r="C70" s="26"/>
+      <c r="A70" s="65" t="s">
+        <v>188</v>
+      </c>
+      <c r="B70" s="66">
+        <v>6</v>
+      </c>
+      <c r="C70" s="66" t="s">
+        <v>8</v>
+      </c>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
       <c r="F70" s="92" t="s">
-        <v>165</v>
+        <v>136</v>
       </c>
       <c r="G70" s="93"/>
       <c r="H70" s="85" t="s">
-        <v>166</v>
+        <v>137</v>
       </c>
       <c r="I70" s="86">
         <v>0.15</v>
       </c>
       <c r="J70" s="87">
         <f t="shared" si="5"/>
-        <v>2450.1999374999996</v>
+        <v>2583.6854062499992</v>
       </c>
       <c r="K70" s="87">
         <f t="shared" si="4"/>
-        <v>306.27499218749995</v>
+        <v>322.9606757812499</v>
       </c>
     </row>
     <row r="71" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="27" t="s">
-        <v>139</v>
-      </c>
-      <c r="B71" s="19">
-        <v>11</v>
-      </c>
-      <c r="C71" s="28" t="s">
-        <v>36</v>
+      <c r="A71" s="65" t="s">
+        <v>189</v>
+      </c>
+      <c r="B71" s="66">
+        <v>6</v>
+      </c>
+      <c r="C71" s="66" t="s">
+        <v>8</v>
       </c>
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
       <c r="F71" s="94" t="s">
-        <v>168</v>
+        <v>139</v>
       </c>
       <c r="G71" s="95">
         <f>H11*G68</f>
-        <v>6533.8664999999992</v>
+        <v>6889.8277499999986</v>
       </c>
       <c r="H71" s="85"/>
       <c r="I71" s="9"/>
       <c r="J71" s="96" t="s">
-        <v>169</v>
+        <v>140</v>
       </c>
       <c r="K71" s="97">
         <f>SUM(K66:K70)</f>
-        <v>2041.8332812499998</v>
+        <v>2153.0711718749994</v>
       </c>
     </row>
     <row r="72" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="73" t="s">
-        <v>140</v>
-      </c>
-      <c r="B72" s="19">
-        <v>9</v>
-      </c>
-      <c r="C72" s="28" t="s">
-        <v>36</v>
+      <c r="A72" s="65" t="s">
+        <v>190</v>
+      </c>
+      <c r="B72" s="45">
+        <v>4</v>
+      </c>
+      <c r="C72" s="98" t="s">
+        <v>8</v>
       </c>
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
@@ -3219,14 +3352,14 @@
       <c r="K72" s="3"/>
     </row>
     <row r="73" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="27" t="s">
-        <v>141</v>
-      </c>
-      <c r="B73" s="19">
-        <v>6</v>
-      </c>
-      <c r="C73" s="28" t="s">
-        <v>62</v>
+      <c r="A73" s="65" t="s">
+        <v>191</v>
+      </c>
+      <c r="B73" s="66">
+        <v>6</v>
+      </c>
+      <c r="C73" s="66" t="s">
+        <v>8</v>
       </c>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
@@ -3238,90 +3371,94 @@
       <c r="K73" s="3"/>
     </row>
     <row r="74" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="45" t="s">
-        <v>142</v>
-      </c>
-      <c r="B74" s="45">
-        <v>10</v>
-      </c>
-      <c r="C74" s="45" t="s">
-        <v>36</v>
+      <c r="A74" s="65" t="s">
+        <v>194</v>
+      </c>
+      <c r="B74" s="66">
+        <v>3</v>
+      </c>
+      <c r="C74" s="66" t="s">
+        <v>6</v>
       </c>
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
     </row>
     <row r="75" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="51" t="s">
-        <v>143</v>
-      </c>
-      <c r="B75" s="26"/>
-      <c r="C75" s="26"/>
+      <c r="A75" s="65" t="s">
+        <v>193</v>
+      </c>
+      <c r="B75" s="66">
+        <v>3</v>
+      </c>
+      <c r="C75" s="66" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="76" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="27" t="s">
-        <v>144</v>
-      </c>
-      <c r="B76" s="19">
-        <v>8</v>
-      </c>
-      <c r="C76" s="28" t="s">
-        <v>36</v>
+      <c r="A76" s="65" t="s">
+        <v>192</v>
+      </c>
+      <c r="B76" s="66">
+        <v>4</v>
+      </c>
+      <c r="C76" s="66" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="77" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="27" t="s">
-        <v>146</v>
-      </c>
-      <c r="B77" s="19">
-        <v>9</v>
-      </c>
-      <c r="C77" s="28" t="s">
-        <v>36</v>
+      <c r="A77" s="65" t="s">
+        <v>195</v>
+      </c>
+      <c r="B77" s="66">
+        <v>7</v>
+      </c>
+      <c r="C77" s="66" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="78" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="27" t="s">
-        <v>147</v>
-      </c>
-      <c r="B78" s="19">
-        <v>10</v>
-      </c>
-      <c r="C78" s="28" t="s">
-        <v>36</v>
+      <c r="A78" s="65" t="s">
+        <v>196</v>
+      </c>
+      <c r="B78" s="66">
+        <v>2</v>
+      </c>
+      <c r="C78" s="66" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="79" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="27" t="s">
-        <v>153</v>
-      </c>
-      <c r="B79" s="19">
-        <v>11</v>
-      </c>
-      <c r="C79" s="28" t="s">
-        <v>36</v>
+      <c r="A79" s="65" t="s">
+        <v>197</v>
+      </c>
+      <c r="B79" s="66">
+        <v>3</v>
+      </c>
+      <c r="C79" s="66" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="80" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="27" t="s">
-        <v>156</v>
-      </c>
-      <c r="B80" s="19">
-        <v>10</v>
-      </c>
-      <c r="C80" s="28" t="s">
-        <v>36</v>
+      <c r="A80" s="65" t="s">
+        <v>198</v>
+      </c>
+      <c r="B80" s="66">
+        <v>2</v>
+      </c>
+      <c r="C80" s="66" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="81" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="51" t="s">
-        <v>159</v>
+        <v>115</v>
       </c>
       <c r="B81" s="26"/>
       <c r="C81" s="26"/>
     </row>
     <row r="82" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="27" t="s">
-        <v>162</v>
+        <v>116</v>
       </c>
       <c r="B82" s="19">
         <v>10</v>
@@ -3331,58 +3468,58 @@
       </c>
     </row>
     <row r="83" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="27" t="s">
-        <v>164</v>
+      <c r="A83" s="73" t="s">
+        <v>199</v>
       </c>
       <c r="B83" s="19">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C83" s="28" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="84" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="27" t="s">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="B84" s="19">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C84" s="28" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="85" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="27" t="s">
-        <v>170</v>
-      </c>
-      <c r="B85" s="19">
-        <v>8</v>
-      </c>
-      <c r="C85" s="28" t="s">
-        <v>11</v>
+      <c r="A85" s="98" t="s">
+        <v>117</v>
+      </c>
+      <c r="B85" s="45">
+        <v>3</v>
+      </c>
+      <c r="C85" s="98" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="86" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="27" t="s">
-        <v>171</v>
-      </c>
-      <c r="B86" s="19">
-        <v>3</v>
+      <c r="A86" s="98" t="s">
+        <v>201</v>
+      </c>
+      <c r="B86" s="106">
+        <v>2</v>
       </c>
       <c r="C86" s="28" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="87" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="27" t="s">
-        <v>172</v>
-      </c>
-      <c r="B87" s="19">
-        <v>3</v>
+      <c r="A87" s="98" t="s">
+        <v>202</v>
+      </c>
+      <c r="B87" s="106">
+        <v>2</v>
       </c>
       <c r="C87" s="28" t="s">
-        <v>136</v>
+        <v>6</v>
       </c>
       <c r="F87" s="3"/>
       <c r="G87" s="3"/>
@@ -3392,11 +3529,15 @@
       <c r="K87" s="3"/>
     </row>
     <row r="88" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="51" t="s">
-        <v>173</v>
-      </c>
-      <c r="B88" s="26"/>
-      <c r="C88" s="26"/>
+      <c r="A88" s="98" t="s">
+        <v>203</v>
+      </c>
+      <c r="B88" s="106">
+        <v>2</v>
+      </c>
+      <c r="C88" s="28" t="s">
+        <v>6</v>
+      </c>
       <c r="D88" s="3"/>
       <c r="F88" s="3"/>
       <c r="G88" s="3"/>
@@ -3406,15 +3547,11 @@
       <c r="K88" s="3"/>
     </row>
     <row r="89" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="98" t="s">
-        <v>174</v>
-      </c>
-      <c r="B89" s="98">
-        <v>9</v>
-      </c>
-      <c r="C89" s="98" t="s">
-        <v>36</v>
-      </c>
+      <c r="A89" s="51" t="s">
+        <v>118</v>
+      </c>
+      <c r="B89" s="26"/>
+      <c r="C89" s="26"/>
       <c r="D89" s="3"/>
       <c r="F89" s="3"/>
       <c r="G89" s="3"/>
@@ -3424,14 +3561,14 @@
       <c r="K89" s="3"/>
     </row>
     <row r="90" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="98" t="s">
-        <v>175</v>
-      </c>
-      <c r="B90" s="98">
-        <v>13</v>
-      </c>
-      <c r="C90" s="98" t="s">
-        <v>36</v>
+      <c r="A90" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="B90" s="19">
+        <v>8</v>
+      </c>
+      <c r="C90" s="28" t="s">
+        <v>11</v>
       </c>
       <c r="D90" s="3"/>
       <c r="F90" s="3"/>
@@ -3442,168 +3579,416 @@
       <c r="K90" s="3"/>
     </row>
     <row r="91" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="98" t="s">
-        <v>176</v>
-      </c>
-      <c r="B91" s="98">
-        <v>6</v>
-      </c>
-      <c r="C91" s="98" t="s">
-        <v>62</v>
+      <c r="A91" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="B91" s="19">
+        <v>9</v>
+      </c>
+      <c r="C91" s="28" t="s">
+        <v>11</v>
       </c>
       <c r="J91" s="3"/>
       <c r="K91" s="3"/>
     </row>
     <row r="92" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="51" t="s">
-        <v>177</v>
-      </c>
-      <c r="B92" s="26"/>
-      <c r="C92" s="26"/>
+      <c r="A92" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="B92" s="19">
+        <v>10</v>
+      </c>
+      <c r="C92" s="28" t="s">
+        <v>11</v>
+      </c>
       <c r="J92" s="3"/>
       <c r="K92" s="3"/>
     </row>
     <row r="93" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="98" t="s">
-        <v>178</v>
-      </c>
-      <c r="B93" s="98">
+      <c r="A93" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="B93" s="19">
         <v>11</v>
       </c>
-      <c r="C93" s="98" t="s">
-        <v>36</v>
+      <c r="C93" s="28" t="s">
+        <v>11</v>
       </c>
       <c r="J93" s="3"/>
       <c r="K93" s="3"/>
     </row>
     <row r="94" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="98" t="s">
-        <v>179</v>
-      </c>
-      <c r="B94" s="98">
+      <c r="A94" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="B94" s="19">
+        <v>10</v>
+      </c>
+      <c r="C94" s="28" t="s">
         <v>11</v>
-      </c>
-      <c r="C94" s="98" t="s">
-        <v>36</v>
       </c>
       <c r="J94" s="3"/>
       <c r="K94" s="3"/>
     </row>
     <row r="95" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="98" t="s">
-        <v>180</v>
-      </c>
-      <c r="B95" s="98">
-        <v>5</v>
-      </c>
-      <c r="C95" s="98" t="s">
-        <v>181</v>
-      </c>
+      <c r="A95" s="51" t="s">
+        <v>206</v>
+      </c>
+      <c r="B95" s="26"/>
+      <c r="C95" s="26"/>
       <c r="J95" s="3"/>
       <c r="K95" s="3"/>
     </row>
     <row r="96" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="51" t="s">
-        <v>182</v>
-      </c>
-      <c r="B96" s="26"/>
-      <c r="C96" s="26"/>
+      <c r="A96" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="B96" s="19">
+        <v>7</v>
+      </c>
+      <c r="C96" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="J96" s="3"/>
       <c r="K96" s="3"/>
     </row>
     <row r="97" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="98" t="s">
-        <v>183</v>
-      </c>
-      <c r="B97" s="98">
-        <v>8</v>
-      </c>
-      <c r="C97" s="98" t="s">
-        <v>36</v>
+      <c r="A97" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="B97" s="19">
+        <v>4</v>
+      </c>
+      <c r="C97" s="28" t="s">
+        <v>8</v>
       </c>
       <c r="J97" s="3"/>
       <c r="K97" s="3"/>
     </row>
     <row r="98" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="98" t="s">
-        <v>184</v>
-      </c>
-      <c r="B98" s="98">
+      <c r="A98" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="B98" s="19">
         <v>4</v>
       </c>
-      <c r="C98" s="98" t="s">
-        <v>62</v>
+      <c r="C98" s="28" t="s">
+        <v>8</v>
       </c>
       <c r="J98" s="3"/>
       <c r="K98" s="3"/>
     </row>
     <row r="99" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="98" t="s">
-        <v>185</v>
-      </c>
-      <c r="B99" s="98">
-        <v>10</v>
-      </c>
-      <c r="C99" s="45" t="s">
-        <v>36</v>
+      <c r="A99" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="B99" s="19">
+        <v>4</v>
+      </c>
+      <c r="C99" s="28" t="s">
+        <v>8</v>
       </c>
       <c r="J99" s="3"/>
       <c r="K99" s="3"/>
     </row>
     <row r="100" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="98" t="s">
-        <v>186</v>
-      </c>
-      <c r="B100" s="98">
-        <v>5</v>
-      </c>
-      <c r="C100" s="45" t="s">
-        <v>62</v>
+      <c r="A100" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="B100" s="19">
+        <v>3</v>
+      </c>
+      <c r="C100" s="28" t="s">
+        <v>6</v>
       </c>
       <c r="J100" s="3"/>
       <c r="K100" s="3"/>
     </row>
     <row r="101" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="98" t="s">
-        <v>187</v>
-      </c>
-      <c r="B101" s="98">
-        <v>3</v>
-      </c>
-      <c r="C101" s="45" t="s">
-        <v>136</v>
-      </c>
+      <c r="A101" s="51" t="s">
+        <v>143</v>
+      </c>
+      <c r="B101" s="26"/>
+      <c r="C101" s="26"/>
       <c r="J101" s="3"/>
       <c r="K101" s="3"/>
     </row>
     <row r="102" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="98" t="s">
-        <v>188</v>
+        <v>144</v>
       </c>
       <c r="B102" s="98">
-        <v>5</v>
-      </c>
-      <c r="C102" s="45" t="s">
-        <v>62</v>
+        <v>7</v>
+      </c>
+      <c r="C102" s="98" t="s">
+        <v>8</v>
       </c>
       <c r="J102" s="3"/>
       <c r="K102" s="3"/>
     </row>
     <row r="103" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="3"/>
-      <c r="B103" s="3"/>
+      <c r="A103" s="98" t="s">
+        <v>208</v>
+      </c>
+      <c r="B103" s="98">
+        <v>8</v>
+      </c>
+      <c r="C103" s="98" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="104" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="3"/>
-      <c r="B104" s="3"/>
+      <c r="A104" s="98" t="s">
+        <v>209</v>
+      </c>
+      <c r="B104" s="98">
+        <v>8</v>
+      </c>
+      <c r="C104" s="98" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="105" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="3"/>
-      <c r="B105" s="3"/>
+      <c r="A105" s="98" t="s">
+        <v>210</v>
+      </c>
+      <c r="B105" s="28">
+        <v>4</v>
+      </c>
+      <c r="C105" s="28" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="106" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="3"/>
-      <c r="B106" s="3"/>
+      <c r="A106" s="98" t="s">
+        <v>211</v>
+      </c>
+      <c r="B106" s="28">
+        <v>2</v>
+      </c>
+      <c r="C106" s="28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="98" t="s">
+        <v>212</v>
+      </c>
+      <c r="B107" s="28">
+        <v>2</v>
+      </c>
+      <c r="C107" s="28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="51" t="s">
+        <v>145</v>
+      </c>
+      <c r="B108" s="26"/>
+      <c r="C108" s="26"/>
+    </row>
+    <row r="109" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="98" t="s">
+        <v>146</v>
+      </c>
+      <c r="B109" s="98">
+        <v>7</v>
+      </c>
+      <c r="C109" s="98" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="98" t="s">
+        <v>213</v>
+      </c>
+      <c r="B110" s="98">
+        <v>4</v>
+      </c>
+      <c r="C110" s="98" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="98" t="s">
+        <v>214</v>
+      </c>
+      <c r="B111" s="98">
+        <v>5</v>
+      </c>
+      <c r="C111" s="98" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="98" t="s">
+        <v>215</v>
+      </c>
+      <c r="B112" s="28">
+        <v>6</v>
+      </c>
+      <c r="C112" s="28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="98" t="s">
+        <v>216</v>
+      </c>
+      <c r="B113" s="28">
+        <v>4</v>
+      </c>
+      <c r="C113" s="28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="98" t="s">
+        <v>217</v>
+      </c>
+      <c r="B114" s="28">
+        <v>5</v>
+      </c>
+      <c r="C114" s="28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="98" t="s">
+        <v>218</v>
+      </c>
+      <c r="B115" s="28">
+        <v>2</v>
+      </c>
+      <c r="C115" s="28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="98" t="s">
+        <v>219</v>
+      </c>
+      <c r="B116" s="28">
+        <v>2</v>
+      </c>
+      <c r="C116" s="28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="98" t="s">
+        <v>220</v>
+      </c>
+      <c r="B117" s="28">
+        <v>2</v>
+      </c>
+      <c r="C117" s="28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="51" t="s">
+        <v>147</v>
+      </c>
+      <c r="B118" s="26"/>
+      <c r="C118" s="26"/>
+    </row>
+    <row r="119" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="98" t="s">
+        <v>148</v>
+      </c>
+      <c r="B119" s="98">
+        <v>6</v>
+      </c>
+      <c r="C119" s="98" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="98" t="s">
+        <v>221</v>
+      </c>
+      <c r="B120" s="98">
+        <v>4</v>
+      </c>
+      <c r="C120" s="98" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="98" t="s">
+        <v>222</v>
+      </c>
+      <c r="B121" s="98">
+        <v>2</v>
+      </c>
+      <c r="C121" s="98" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="98" t="s">
+        <v>223</v>
+      </c>
+      <c r="B122" s="98">
+        <v>2</v>
+      </c>
+      <c r="C122" s="98" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="98" t="s">
+        <v>224</v>
+      </c>
+      <c r="B123" s="98">
+        <v>5</v>
+      </c>
+      <c r="C123" s="98" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="107" t="s">
+        <v>225</v>
+      </c>
+      <c r="B124" s="107">
+        <v>2</v>
+      </c>
+      <c r="C124" s="107" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="108" t="s">
+        <v>226</v>
+      </c>
+      <c r="B125" s="108">
+        <v>3</v>
+      </c>
+      <c r="C125" s="109" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="108" t="s">
+        <v>149</v>
+      </c>
+      <c r="B126" s="108">
+        <v>2</v>
+      </c>
+      <c r="C126" s="109" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="3"/>
+      <c r="B127" s="3"/>
+    </row>
+    <row r="128" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A128" s="3"/>
+      <c r="B128" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>